<commit_message>
bbox imagenes segementadas RE
</commit_message>
<xml_diff>
--- a/TODAAS/ambas.xlsx
+++ b/TODAAS/ambas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>00004_batch2.jpg</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>00054.jpg</t>
-  </si>
-  <si>
-    <t>00063_batch2.jpg</t>
   </si>
   <si>
     <t>00064_batch2.jpg</t>
@@ -578,7 +575,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B70"/>
+  <dimension ref="A1:B69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1133,14 +1130,6 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
-      <c r="A70" s="1">
-        <v>68</v>
-      </c>
-      <c r="B70" t="s">
-        <v>68</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>